<commit_message>
Rebrand application from "Idea2Solution" to "Ideen-Portal | St. Galler Stadtwerke" with SGSW logo integration
- Updated page metadata title from "Idea2Solution" to "Ideen-Portal | St. Galler Stadtwerke"
- Extended metadata description to include "St. Galler Stadtwerke" organization name
- Changed homepage heading from "Idea2Solution" to "Ideen-Portal" with subtitle "der St. Galler Stadtwerke"
- Replaced Lightbulb icon with SgswLogo component in Navbar (28x28px)
- Updated Navbar app name display
</commit_message>
<xml_diff>
--- a/docs/datenfelder.xlsx
+++ b/docs/datenfelder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianbrunner/repos/idea-to-solution-platform/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7233DD1-F549-B14D-9282-7B3F224368D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C94FBD-932D-A846-9EB5-9B147B798A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18380" yWindow="880" windowWidth="17620" windowHeight="19140" xr2:uid="{D7902B05-8DA2-A448-9DB3-28B1B6EA6B2B}"/>
+    <workbookView xWindow="840" yWindow="880" windowWidth="35160" windowHeight="19140" xr2:uid="{D7902B05-8DA2-A448-9DB3-28B1B6EA6B2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -912,23 +912,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -936,18 +924,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1290,8 +1289,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13D2274-C069-294E-A343-6EEC397EE88E}">
   <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75:D76"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1304,318 +1304,283 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="17"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="18" t="s">
+      <c r="A8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="18" t="s">
+      <c r="A9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15" t="s">
+      <c r="A10" s="10"/>
+      <c r="D10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="26" t="s">
+      <c r="A11" s="10"/>
+      <c r="D11" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="26" t="s">
+      <c r="A12" s="10"/>
+      <c r="D12" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
+      <c r="A13" s="10"/>
+      <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
+      <c r="A14" s="10"/>
+      <c r="D14" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
+      <c r="A15" s="10"/>
+      <c r="D15" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15" t="s">
+      <c r="A16" s="10"/>
+      <c r="D16" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="21"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
+      <c r="A20" s="16"/>
+      <c r="D20" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="18" t="s">
+      <c r="A21" s="16"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="18" t="s">
+      <c r="A22" s="16"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15" t="s">
+      <c r="A23" s="16"/>
+      <c r="D23" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="26" t="s">
+      <c r="A24" s="16"/>
+      <c r="D24" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="26" t="s">
+      <c r="A25" s="16"/>
+      <c r="D25" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15" t="s">
+      <c r="A26" s="16"/>
+      <c r="D26" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15" t="s">
+      <c r="A27" s="16"/>
+      <c r="D27" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15" t="s">
+      <c r="A28" s="16"/>
+      <c r="D28" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="21"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15" t="s">
+      <c r="A29" s="16"/>
+      <c r="D29" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="22"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11" t="s">
+      <c r="A30" s="17"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1623,138 +1588,121 @@
       <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9" t="s">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="21"/>
-      <c r="B33" s="15" t="s">
+      <c r="A33" s="16"/>
+      <c r="B33" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="21"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="18" t="s">
+      <c r="A34" s="16"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="21"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="18" t="s">
+      <c r="A35" s="16"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="21"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15" t="s">
+      <c r="A36" s="16"/>
+      <c r="D36" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="21"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="26" t="s">
+      <c r="A37" s="16"/>
+      <c r="D37" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="21"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="26" t="s">
+      <c r="A38" s="16"/>
+      <c r="D38" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="21"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15" t="s">
+      <c r="A39" s="16"/>
+      <c r="D39" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="21"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15" t="s">
+      <c r="A40" s="16"/>
+      <c r="D40" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="21"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15" t="s">
+      <c r="A41" s="16"/>
+      <c r="D41" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="21"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15" t="s">
+      <c r="A42" s="16"/>
+      <c r="D42" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="E42" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="22"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11" t="s">
+      <c r="A43" s="17"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1762,191 +1710,163 @@
       <c r="A44" s="1"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9" t="s">
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="21"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15" t="s">
+      <c r="A46" s="16"/>
+      <c r="D46" t="s">
         <v>1</v>
       </c>
-      <c r="E46" s="19" t="s">
+      <c r="E46" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="21"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="18" t="s">
+      <c r="A47" s="16"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="19" t="s">
+      <c r="E47" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="21"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="18" t="s">
+      <c r="A48" s="16"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E48" s="19" t="s">
+      <c r="E48" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="21"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15" t="s">
+      <c r="A49" s="16"/>
+      <c r="D49" t="s">
         <v>3</v>
       </c>
-      <c r="E49" s="19" t="s">
+      <c r="E49" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="21"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="26" t="s">
+      <c r="A50" s="16"/>
+      <c r="D50" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E50" s="19" t="s">
+      <c r="E50" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="21"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="26" t="s">
+      <c r="A51" s="16"/>
+      <c r="D51" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E51" s="19" t="s">
+      <c r="E51" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="21"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="20" t="s">
+      <c r="A52" s="16"/>
+      <c r="D52" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E52" s="19" t="s">
+      <c r="E52" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="21"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="20" t="s">
+      <c r="A53" s="16"/>
+      <c r="D53" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="19" t="s">
+      <c r="E53" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="21"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="20" t="s">
+      <c r="A54" s="16"/>
+      <c r="D54" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E54" s="19" t="s">
+      <c r="E54" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="21"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="23" t="s">
+      <c r="A55" s="16"/>
+      <c r="D55" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E55" s="19" t="s">
+      <c r="E55" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="21"/>
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="23" t="s">
+      <c r="A56" s="16"/>
+      <c r="D56" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E56" s="19" t="s">
+      <c r="E56" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="21"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15" t="s">
+      <c r="A57" s="16"/>
+      <c r="D57" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="19" t="s">
+      <c r="E57" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="21"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15" t="s">
+      <c r="A58" s="16"/>
+      <c r="D58" t="s">
         <v>7</v>
       </c>
-      <c r="E58" s="19" t="s">
+      <c r="E58" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="21"/>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15" t="s">
+      <c r="A59" s="16"/>
+      <c r="D59" t="s">
         <v>2</v>
       </c>
-      <c r="E59" s="19" t="s">
+      <c r="E59" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="21"/>
-      <c r="B60" s="15"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15" t="s">
+      <c r="A60" s="16"/>
+      <c r="D60" t="s">
         <v>8</v>
       </c>
-      <c r="E60" s="19" t="s">
+      <c r="E60" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="22"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11" t="s">
+      <c r="A61" s="17"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E61" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1954,1635 +1874,1370 @@
       <c r="A62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9" t="s">
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="E63" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="21"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15" t="s">
+      <c r="A64" s="16"/>
+      <c r="D64" t="s">
         <v>1</v>
       </c>
-      <c r="E64" s="19" t="s">
+      <c r="E64" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="21"/>
-      <c r="B65" s="15"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="18" t="s">
+      <c r="A65" s="16"/>
+      <c r="D65" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E65" s="19" t="s">
+      <c r="E65" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="21"/>
-      <c r="B66" s="15"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="18" t="s">
+      <c r="A66" s="16"/>
+      <c r="D66" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E66" s="19" t="s">
+      <c r="E66" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="21"/>
-      <c r="B67" s="15"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15" t="s">
+      <c r="A67" s="16"/>
+      <c r="D67" t="s">
         <v>3</v>
       </c>
-      <c r="E67" s="19" t="s">
+      <c r="E67" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="21"/>
-      <c r="B68" s="15"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="26" t="s">
+      <c r="A68" s="16"/>
+      <c r="D68" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E68" s="19" t="s">
+      <c r="E68" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="21"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="26" t="s">
+      <c r="A69" s="16"/>
+      <c r="D69" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E69" s="19" t="s">
+      <c r="E69" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="21"/>
-      <c r="B70" s="15"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="20" t="s">
+      <c r="A70" s="16"/>
+      <c r="D70" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E70" s="19" t="s">
+      <c r="E70" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="21"/>
-      <c r="B71" s="15"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="20" t="s">
+      <c r="A71" s="16"/>
+      <c r="D71" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E71" s="19" t="s">
+      <c r="E71" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="21"/>
-      <c r="B72" s="15"/>
-      <c r="C72" s="15"/>
-      <c r="D72" s="20" t="s">
+      <c r="A72" s="16"/>
+      <c r="D72" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E72" s="19" t="s">
+      <c r="E72" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="21"/>
-      <c r="B73" s="15"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="23" t="s">
+      <c r="A73" s="16"/>
+      <c r="D73" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E73" s="19" t="s">
+      <c r="E73" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="21"/>
-      <c r="B74" s="15"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="23" t="s">
+      <c r="A74" s="16"/>
+      <c r="D74" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E74" s="19" t="s">
+      <c r="E74" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="21"/>
-      <c r="B75" s="15"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="24" t="s">
+      <c r="A75" s="16"/>
+      <c r="D75" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E75" s="19" t="s">
+      <c r="E75" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="21"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="15"/>
-      <c r="D76" s="24" t="s">
+      <c r="A76" s="16"/>
+      <c r="D76" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E76" s="19" t="s">
+      <c r="E76" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="21"/>
-      <c r="B77" s="15"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15" t="s">
+      <c r="A77" s="16"/>
+      <c r="D77" t="s">
         <v>6</v>
       </c>
-      <c r="E77" s="19" t="s">
+      <c r="E77" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="14"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15" t="s">
+      <c r="A78" s="10"/>
+      <c r="D78" t="s">
         <v>7</v>
       </c>
-      <c r="E78" s="19" t="s">
+      <c r="E78" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="14"/>
-      <c r="B79" s="15"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15" t="s">
+      <c r="A79" s="10"/>
+      <c r="D79" t="s">
         <v>2</v>
       </c>
-      <c r="E79" s="19" t="s">
+      <c r="E79" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="14"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15" t="s">
+      <c r="A80" s="10"/>
+      <c r="D80" t="s">
         <v>8</v>
       </c>
-      <c r="E80" s="19" t="s">
+      <c r="E80" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="4"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11" t="s">
+      <c r="A81" s="2"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E81" s="12" t="s">
+      <c r="E81" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="13" t="s">
+      <c r="A83" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B83" s="9"/>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9" t="s">
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E83" s="10" t="s">
+      <c r="E83" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="14"/>
-      <c r="B84" s="15"/>
-      <c r="C84" s="15"/>
-      <c r="D84" s="15" t="s">
+      <c r="A84" s="10"/>
+      <c r="D84" t="s">
         <v>1</v>
       </c>
-      <c r="E84" s="19" t="s">
+      <c r="E84" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="14"/>
-      <c r="B85" s="15"/>
-      <c r="C85" s="15"/>
-      <c r="D85" s="18" t="s">
+      <c r="A85" s="10"/>
+      <c r="D85" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E85" s="19" t="s">
+      <c r="E85" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="14"/>
-      <c r="B86" s="15"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="18" t="s">
+      <c r="A86" s="10"/>
+      <c r="D86" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E86" s="19" t="s">
+      <c r="E86" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="14"/>
-      <c r="B87" s="15"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="15" t="s">
+      <c r="A87" s="10"/>
+      <c r="D87" t="s">
         <v>3</v>
       </c>
-      <c r="E87" s="19" t="s">
+      <c r="E87" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" s="14"/>
-      <c r="B88" s="15"/>
-      <c r="C88" s="15"/>
-      <c r="D88" s="26" t="s">
+      <c r="A88" s="10"/>
+      <c r="D88" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E88" s="19" t="s">
+      <c r="E88" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" s="14"/>
-      <c r="B89" s="15"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="26" t="s">
+      <c r="A89" s="10"/>
+      <c r="D89" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E89" s="19" t="s">
+      <c r="E89" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="14"/>
-      <c r="B90" s="15"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="20" t="s">
+      <c r="A90" s="10"/>
+      <c r="D90" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E90" s="19" t="s">
+      <c r="E90" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" s="14"/>
-      <c r="B91" s="15"/>
-      <c r="C91" s="15"/>
-      <c r="D91" s="20" t="s">
+      <c r="A91" s="10"/>
+      <c r="D91" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E91" s="19" t="s">
+      <c r="E91" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" s="14"/>
-      <c r="B92" s="15"/>
-      <c r="C92" s="15"/>
-      <c r="D92" s="20" t="s">
+      <c r="A92" s="10"/>
+      <c r="D92" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E92" s="19" t="s">
+      <c r="E92" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="14"/>
-      <c r="B93" s="15"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="23" t="s">
+      <c r="A93" s="10"/>
+      <c r="D93" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E93" s="19" t="s">
+      <c r="E93" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="14"/>
-      <c r="B94" s="15"/>
-      <c r="C94" s="15"/>
-      <c r="D94" s="23" t="s">
+      <c r="A94" s="10"/>
+      <c r="D94" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E94" s="19" t="s">
+      <c r="E94" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" s="14"/>
-      <c r="B95" s="15"/>
-      <c r="C95" s="15"/>
-      <c r="D95" s="24" t="s">
+      <c r="A95" s="10"/>
+      <c r="D95" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E95" s="19" t="s">
+      <c r="E95" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" s="14"/>
-      <c r="B96" s="15"/>
-      <c r="C96" s="15"/>
-      <c r="D96" s="24" t="s">
+      <c r="A96" s="10"/>
+      <c r="D96" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E96" s="19" t="s">
+      <c r="E96" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97" s="14"/>
-      <c r="B97" s="15"/>
-      <c r="C97" s="15"/>
-      <c r="D97" s="25" t="s">
+      <c r="A97" s="10"/>
+      <c r="D97" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E97" s="19" t="s">
+      <c r="E97" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98" s="14"/>
-      <c r="B98" s="15"/>
-      <c r="C98" s="15"/>
-      <c r="D98" s="25" t="s">
+      <c r="A98" s="10"/>
+      <c r="D98" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E98" s="19" t="s">
+      <c r="E98" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="14"/>
-      <c r="B99" s="15"/>
-      <c r="C99" s="15"/>
-      <c r="D99" s="15" t="s">
+      <c r="A99" s="10"/>
+      <c r="D99" t="s">
         <v>6</v>
       </c>
-      <c r="E99" s="19" t="s">
+      <c r="E99" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100" s="14"/>
-      <c r="B100" s="15"/>
-      <c r="C100" s="15"/>
-      <c r="D100" s="15" t="s">
+      <c r="A100" s="10"/>
+      <c r="D100" t="s">
         <v>7</v>
       </c>
-      <c r="E100" s="19" t="s">
+      <c r="E100" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101" s="14"/>
-      <c r="B101" s="15"/>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15" t="s">
+      <c r="A101" s="10"/>
+      <c r="D101" t="s">
         <v>2</v>
       </c>
-      <c r="E101" s="19" t="s">
+      <c r="E101" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" s="14"/>
-      <c r="B102" s="15"/>
-      <c r="C102" s="15"/>
-      <c r="D102" s="15" t="s">
+      <c r="A102" s="10"/>
+      <c r="D102" t="s">
         <v>8</v>
       </c>
-      <c r="E102" s="19" t="s">
+      <c r="E102" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103" s="4"/>
-      <c r="B103" s="11"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11" t="s">
+      <c r="A103" s="2"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E103" s="12" t="s">
+      <c r="E103" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105" s="13" t="s">
+      <c r="A105" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B105" s="9"/>
-      <c r="C105" s="9"/>
-      <c r="D105" s="9" t="s">
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E105" s="10" t="s">
+      <c r="E105" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106" s="14"/>
-      <c r="B106" s="15"/>
-      <c r="C106" s="15"/>
-      <c r="D106" s="15" t="s">
+      <c r="A106" s="10"/>
+      <c r="D106" t="s">
         <v>1</v>
       </c>
-      <c r="E106" s="19" t="s">
+      <c r="E106" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107" s="14"/>
-      <c r="B107" s="15"/>
-      <c r="C107" s="15"/>
-      <c r="D107" s="18" t="s">
+      <c r="A107" s="10"/>
+      <c r="D107" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E107" s="19" t="s">
+      <c r="E107" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108" s="14"/>
-      <c r="B108" s="15"/>
-      <c r="C108" s="15"/>
-      <c r="D108" s="18" t="s">
+      <c r="A108" s="10"/>
+      <c r="D108" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E108" s="19" t="s">
+      <c r="E108" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109" s="14"/>
-      <c r="B109" s="15"/>
-      <c r="C109" s="15"/>
-      <c r="D109" s="15" t="s">
+      <c r="A109" s="10"/>
+      <c r="D109" t="s">
         <v>3</v>
       </c>
-      <c r="E109" s="19" t="s">
+      <c r="E109" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110" s="14"/>
-      <c r="B110" s="15"/>
-      <c r="C110" s="15"/>
-      <c r="D110" s="26" t="s">
+      <c r="A110" s="10"/>
+      <c r="D110" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E110" s="19" t="s">
+      <c r="E110" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" s="14"/>
-      <c r="B111" s="15"/>
-      <c r="C111" s="15"/>
-      <c r="D111" s="26" t="s">
+      <c r="A111" s="10"/>
+      <c r="D111" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E111" s="19" t="s">
+      <c r="E111" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112" s="14"/>
-      <c r="B112" s="15"/>
-      <c r="C112" s="15"/>
-      <c r="D112" s="20" t="s">
+      <c r="A112" s="10"/>
+      <c r="D112" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E112" s="19" t="s">
+      <c r="E112" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113" s="14"/>
-      <c r="B113" s="15"/>
-      <c r="C113" s="15"/>
-      <c r="D113" s="20" t="s">
+      <c r="A113" s="10"/>
+      <c r="D113" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E113" s="19" t="s">
+      <c r="E113" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114" s="14"/>
-      <c r="B114" s="15"/>
-      <c r="C114" s="15"/>
-      <c r="D114" s="20" t="s">
+      <c r="A114" s="10"/>
+      <c r="D114" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E114" s="19" t="s">
+      <c r="E114" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115" s="14"/>
-      <c r="B115" s="15"/>
-      <c r="C115" s="15"/>
-      <c r="D115" s="23" t="s">
+      <c r="A115" s="10"/>
+      <c r="D115" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E115" s="19" t="s">
+      <c r="E115" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" s="14"/>
-      <c r="B116" s="15"/>
-      <c r="C116" s="15"/>
-      <c r="D116" s="23" t="s">
+      <c r="A116" s="10"/>
+      <c r="D116" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E116" s="19" t="s">
+      <c r="E116" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" s="14"/>
-      <c r="B117" s="15"/>
-      <c r="C117" s="15"/>
-      <c r="D117" s="24" t="s">
+      <c r="A117" s="10"/>
+      <c r="D117" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E117" s="19" t="s">
+      <c r="E117" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118" s="14"/>
-      <c r="B118" s="15"/>
-      <c r="C118" s="15"/>
-      <c r="D118" s="24" t="s">
+      <c r="A118" s="10"/>
+      <c r="D118" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E118" s="19" t="s">
+      <c r="E118" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119" s="14"/>
-      <c r="B119" s="15"/>
-      <c r="C119" s="15"/>
-      <c r="D119" s="25" t="s">
+      <c r="A119" s="10"/>
+      <c r="D119" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E119" s="19" t="s">
+      <c r="E119" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120" s="14"/>
-      <c r="B120" s="15"/>
-      <c r="C120" s="15"/>
-      <c r="D120" s="25" t="s">
+      <c r="A120" s="10"/>
+      <c r="D120" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E120" s="19" t="s">
+      <c r="E120" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A121" s="14"/>
-      <c r="B121" s="15"/>
-      <c r="C121" s="15"/>
-      <c r="D121" s="15" t="s">
+      <c r="A121" s="10"/>
+      <c r="D121" t="s">
         <v>6</v>
       </c>
-      <c r="E121" s="19" t="s">
+      <c r="E121" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122" s="14"/>
-      <c r="B122" s="15"/>
-      <c r="C122" s="15"/>
-      <c r="D122" s="15" t="s">
+      <c r="A122" s="10"/>
+      <c r="D122" t="s">
         <v>7</v>
       </c>
-      <c r="E122" s="19" t="s">
+      <c r="E122" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123" s="14"/>
-      <c r="B123" s="15"/>
-      <c r="C123" s="15"/>
-      <c r="D123" s="15" t="s">
+      <c r="A123" s="10"/>
+      <c r="D123" t="s">
         <v>2</v>
       </c>
-      <c r="E123" s="19" t="s">
+      <c r="E123" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A124" s="14"/>
-      <c r="B124" s="15"/>
-      <c r="C124" s="15"/>
-      <c r="D124" s="15" t="s">
+      <c r="A124" s="10"/>
+      <c r="D124" t="s">
         <v>8</v>
       </c>
-      <c r="E124" s="19" t="s">
+      <c r="E124" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125" s="4"/>
-      <c r="B125" s="11"/>
-      <c r="C125" s="11"/>
-      <c r="D125" s="11" t="s">
+      <c r="A125" s="2"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="7"/>
+      <c r="D125" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E125" s="12" t="s">
+      <c r="E125" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127" s="13" t="s">
+      <c r="A127" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B127" s="9"/>
-      <c r="C127" s="9"/>
-      <c r="D127" s="9" t="s">
+      <c r="B127" s="5"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E127" s="10" t="s">
+      <c r="E127" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128" s="14"/>
-      <c r="B128" s="15"/>
-      <c r="C128" s="15"/>
-      <c r="D128" s="15" t="s">
+      <c r="A128" s="10"/>
+      <c r="D128" t="s">
         <v>1</v>
       </c>
-      <c r="E128" s="19" t="s">
+      <c r="E128" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A129" s="14"/>
-      <c r="B129" s="15"/>
-      <c r="C129" s="15"/>
-      <c r="D129" s="18" t="s">
+      <c r="A129" s="10"/>
+      <c r="D129" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E129" s="19" t="s">
+      <c r="E129" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130" s="14"/>
-      <c r="B130" s="15"/>
-      <c r="C130" s="15"/>
-      <c r="D130" s="18" t="s">
+      <c r="A130" s="10"/>
+      <c r="D130" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E130" s="19" t="s">
+      <c r="E130" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A131" s="14"/>
-      <c r="B131" s="15"/>
-      <c r="C131" s="15"/>
-      <c r="D131" s="15" t="s">
+      <c r="A131" s="10"/>
+      <c r="D131" t="s">
         <v>3</v>
       </c>
-      <c r="E131" s="19" t="s">
+      <c r="E131" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A132" s="14"/>
-      <c r="B132" s="15"/>
-      <c r="C132" s="15"/>
-      <c r="D132" s="26" t="s">
+      <c r="A132" s="10"/>
+      <c r="D132" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E132" s="19" t="s">
+      <c r="E132" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A133" s="14"/>
-      <c r="B133" s="15"/>
-      <c r="C133" s="15"/>
-      <c r="D133" s="26" t="s">
+      <c r="A133" s="10"/>
+      <c r="D133" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E133" s="19" t="s">
+      <c r="E133" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A134" s="14"/>
-      <c r="B134" s="15"/>
-      <c r="C134" s="15"/>
-      <c r="D134" s="20" t="s">
+      <c r="A134" s="10"/>
+      <c r="D134" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E134" s="19" t="s">
+      <c r="E134" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A135" s="14"/>
-      <c r="B135" s="15"/>
-      <c r="C135" s="15"/>
-      <c r="D135" s="20" t="s">
+      <c r="A135" s="10"/>
+      <c r="D135" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E135" s="19" t="s">
+      <c r="E135" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A136" s="14"/>
-      <c r="B136" s="15"/>
-      <c r="C136" s="15"/>
-      <c r="D136" s="20" t="s">
+      <c r="A136" s="10"/>
+      <c r="D136" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E136" s="19" t="s">
+      <c r="E136" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A137" s="14"/>
-      <c r="B137" s="15"/>
-      <c r="C137" s="15"/>
-      <c r="D137" s="23" t="s">
+      <c r="A137" s="10"/>
+      <c r="D137" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E137" s="19" t="s">
+      <c r="E137" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A138" s="14"/>
-      <c r="B138" s="15"/>
-      <c r="C138" s="15"/>
-      <c r="D138" s="23" t="s">
+      <c r="A138" s="10"/>
+      <c r="D138" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E138" s="19" t="s">
+      <c r="E138" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A139" s="14"/>
-      <c r="B139" s="15"/>
-      <c r="C139" s="15"/>
-      <c r="D139" s="24" t="s">
+      <c r="A139" s="10"/>
+      <c r="D139" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E139" s="19" t="s">
+      <c r="E139" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A140" s="14"/>
-      <c r="B140" s="15"/>
-      <c r="C140" s="15"/>
-      <c r="D140" s="24" t="s">
+      <c r="A140" s="10"/>
+      <c r="D140" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E140" s="19" t="s">
+      <c r="E140" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141" s="14"/>
-      <c r="B141" s="15"/>
-      <c r="C141" s="15"/>
-      <c r="D141" s="25" t="s">
+      <c r="A141" s="10"/>
+      <c r="D141" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E141" s="19" t="s">
+      <c r="E141" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142" s="14"/>
-      <c r="B142" s="15"/>
-      <c r="C142" s="15"/>
-      <c r="D142" s="25" t="s">
+      <c r="A142" s="10"/>
+      <c r="D142" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E142" s="19" t="s">
+      <c r="E142" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A143" s="14"/>
-      <c r="B143" s="15"/>
-      <c r="C143" s="15"/>
-      <c r="D143" s="15" t="s">
+      <c r="A143" s="10"/>
+      <c r="D143" t="s">
         <v>6</v>
       </c>
-      <c r="E143" s="19" t="s">
+      <c r="E143" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A144" s="14"/>
-      <c r="B144" s="15"/>
-      <c r="C144" s="15"/>
-      <c r="D144" s="15" t="s">
+      <c r="A144" s="10"/>
+      <c r="D144" t="s">
         <v>7</v>
       </c>
-      <c r="E144" s="19" t="s">
+      <c r="E144" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A145" s="14"/>
-      <c r="B145" s="15"/>
-      <c r="C145" s="15"/>
-      <c r="D145" s="15" t="s">
+      <c r="A145" s="10"/>
+      <c r="D145" t="s">
         <v>2</v>
       </c>
-      <c r="E145" s="19" t="s">
+      <c r="E145" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A146" s="14"/>
-      <c r="B146" s="15"/>
-      <c r="C146" s="15"/>
-      <c r="D146" s="15" t="s">
+      <c r="A146" s="10"/>
+      <c r="D146" t="s">
         <v>8</v>
       </c>
-      <c r="E146" s="19" t="s">
+      <c r="E146" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147" s="4"/>
-      <c r="B147" s="11"/>
-      <c r="C147" s="11"/>
-      <c r="D147" s="11" t="s">
+      <c r="A147" s="2"/>
+      <c r="B147" s="7"/>
+      <c r="C147" s="7"/>
+      <c r="D147" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E147" s="12" t="s">
+      <c r="E147" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A149" s="13" t="s">
+      <c r="A149" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B149" s="9"/>
-      <c r="C149" s="9"/>
-      <c r="D149" s="9" t="s">
+      <c r="B149" s="5"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E149" s="10" t="s">
+      <c r="E149" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A150" s="14"/>
-      <c r="B150" s="15"/>
-      <c r="C150" s="15"/>
-      <c r="D150" s="15" t="s">
+      <c r="A150" s="10"/>
+      <c r="D150" t="s">
         <v>1</v>
       </c>
-      <c r="E150" s="19" t="s">
+      <c r="E150" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A151" s="14"/>
-      <c r="B151" s="15"/>
-      <c r="C151" s="15"/>
-      <c r="D151" s="18" t="s">
+      <c r="A151" s="10"/>
+      <c r="D151" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E151" s="19" t="s">
+      <c r="E151" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152" s="14"/>
-      <c r="B152" s="15"/>
-      <c r="C152" s="15"/>
-      <c r="D152" s="18" t="s">
+      <c r="A152" s="10"/>
+      <c r="D152" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E152" s="19" t="s">
+      <c r="E152" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A153" s="14"/>
-      <c r="B153" s="15"/>
-      <c r="C153" s="15"/>
-      <c r="D153" s="15" t="s">
+      <c r="A153" s="10"/>
+      <c r="D153" t="s">
         <v>3</v>
       </c>
-      <c r="E153" s="19" t="s">
+      <c r="E153" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A154" s="14"/>
-      <c r="B154" s="15"/>
-      <c r="C154" s="15"/>
-      <c r="D154" s="26" t="s">
+      <c r="A154" s="10"/>
+      <c r="D154" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E154" s="19" t="s">
+      <c r="E154" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A155" s="14"/>
-      <c r="B155" s="15"/>
-      <c r="C155" s="15"/>
-      <c r="D155" s="26" t="s">
+      <c r="A155" s="10"/>
+      <c r="D155" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E155" s="19" t="s">
+      <c r="E155" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A156" s="14"/>
-      <c r="B156" s="15"/>
-      <c r="C156" s="15"/>
-      <c r="D156" s="20" t="s">
+      <c r="A156" s="10"/>
+      <c r="D156" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E156" s="19" t="s">
+      <c r="E156" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A157" s="14"/>
-      <c r="B157" s="15"/>
-      <c r="C157" s="15"/>
-      <c r="D157" s="20" t="s">
+      <c r="A157" s="10"/>
+      <c r="D157" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E157" s="19" t="s">
+      <c r="E157" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A158" s="14"/>
-      <c r="B158" s="15"/>
-      <c r="C158" s="15"/>
-      <c r="D158" s="20" t="s">
+      <c r="A158" s="10"/>
+      <c r="D158" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E158" s="19" t="s">
+      <c r="E158" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A159" s="14"/>
-      <c r="B159" s="15"/>
-      <c r="C159" s="15"/>
-      <c r="D159" s="23" t="s">
+      <c r="A159" s="10"/>
+      <c r="D159" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E159" s="19" t="s">
+      <c r="E159" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A160" s="14"/>
-      <c r="B160" s="15"/>
-      <c r="C160" s="15"/>
-      <c r="D160" s="23" t="s">
+      <c r="A160" s="10"/>
+      <c r="D160" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E160" s="19" t="s">
+      <c r="E160" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A161" s="14"/>
-      <c r="B161" s="15"/>
-      <c r="C161" s="15"/>
-      <c r="D161" s="24" t="s">
+      <c r="A161" s="10"/>
+      <c r="D161" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E161" s="19" t="s">
+      <c r="E161" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A162" s="14"/>
-      <c r="B162" s="15"/>
-      <c r="C162" s="15"/>
-      <c r="D162" s="24" t="s">
+      <c r="A162" s="10"/>
+      <c r="D162" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E162" s="19" t="s">
+      <c r="E162" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A163" s="14"/>
-      <c r="B163" s="15"/>
-      <c r="C163" s="15"/>
-      <c r="D163" s="25" t="s">
+      <c r="A163" s="10"/>
+      <c r="D163" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E163" s="19" t="s">
+      <c r="E163" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A164" s="14"/>
-      <c r="B164" s="15"/>
-      <c r="C164" s="15"/>
-      <c r="D164" s="25" t="s">
+      <c r="A164" s="10"/>
+      <c r="D164" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E164" s="19" t="s">
+      <c r="E164" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A165" s="14"/>
-      <c r="B165" s="15"/>
-      <c r="C165" s="15"/>
-      <c r="D165" s="15" t="s">
+      <c r="A165" s="10"/>
+      <c r="D165" t="s">
         <v>6</v>
       </c>
-      <c r="E165" s="19" t="s">
+      <c r="E165" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A166" s="14"/>
-      <c r="B166" s="15"/>
-      <c r="C166" s="15"/>
-      <c r="D166" s="15" t="s">
+      <c r="A166" s="10"/>
+      <c r="D166" t="s">
         <v>7</v>
       </c>
-      <c r="E166" s="19" t="s">
+      <c r="E166" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A167" s="14"/>
-      <c r="B167" s="15"/>
-      <c r="C167" s="15"/>
-      <c r="D167" s="15" t="s">
+      <c r="A167" s="10"/>
+      <c r="D167" t="s">
         <v>2</v>
       </c>
-      <c r="E167" s="19" t="s">
+      <c r="E167" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A168" s="14"/>
-      <c r="B168" s="15"/>
-      <c r="C168" s="15"/>
-      <c r="D168" s="15" t="s">
+      <c r="A168" s="10"/>
+      <c r="D168" t="s">
         <v>8</v>
       </c>
-      <c r="E168" s="19" t="s">
+      <c r="E168" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A169" s="4"/>
-      <c r="B169" s="11"/>
-      <c r="C169" s="11"/>
-      <c r="D169" s="11" t="s">
+      <c r="A169" s="2"/>
+      <c r="B169" s="7"/>
+      <c r="C169" s="7"/>
+      <c r="D169" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E169" s="12" t="s">
+      <c r="E169" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A171" s="13" t="s">
+      <c r="A171" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B171" s="9"/>
-      <c r="C171" s="9"/>
-      <c r="D171" s="9" t="s">
+      <c r="B171" s="5"/>
+      <c r="C171" s="5"/>
+      <c r="D171" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E171" s="10" t="s">
+      <c r="E171" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A172" s="14"/>
-      <c r="B172" s="15"/>
-      <c r="C172" s="15"/>
-      <c r="D172" s="15" t="s">
+      <c r="A172" s="10"/>
+      <c r="D172" t="s">
         <v>1</v>
       </c>
-      <c r="E172" s="19" t="s">
+      <c r="E172" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A173" s="21"/>
-      <c r="B173" s="15"/>
-      <c r="C173" s="15"/>
-      <c r="D173" s="18" t="s">
+      <c r="A173" s="16"/>
+      <c r="D173" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E173" s="19" t="s">
+      <c r="E173" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A174" s="14"/>
-      <c r="B174" s="15"/>
-      <c r="C174" s="15"/>
-      <c r="D174" s="18" t="s">
+      <c r="A174" s="10"/>
+      <c r="D174" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E174" s="19" t="s">
+      <c r="E174" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A175" s="14"/>
-      <c r="B175" s="15"/>
-      <c r="C175" s="15"/>
-      <c r="D175" s="15" t="s">
+      <c r="A175" s="10"/>
+      <c r="D175" t="s">
         <v>3</v>
       </c>
-      <c r="E175" s="19" t="s">
+      <c r="E175" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A176" s="14"/>
-      <c r="B176" s="15"/>
-      <c r="C176" s="15"/>
-      <c r="D176" s="26" t="s">
+      <c r="A176" s="10"/>
+      <c r="D176" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E176" s="19" t="s">
+      <c r="E176" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A177" s="14"/>
-      <c r="B177" s="15"/>
-      <c r="C177" s="15"/>
-      <c r="D177" s="26" t="s">
+      <c r="A177" s="10"/>
+      <c r="D177" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E177" s="19" t="s">
+      <c r="E177" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A178" s="14"/>
-      <c r="B178" s="15"/>
-      <c r="C178" s="15"/>
-      <c r="D178" s="20" t="s">
+      <c r="A178" s="10"/>
+      <c r="D178" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E178" s="19" t="s">
+      <c r="E178" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A179" s="14"/>
-      <c r="B179" s="15"/>
-      <c r="C179" s="15"/>
-      <c r="D179" s="20" t="s">
+      <c r="A179" s="10"/>
+      <c r="D179" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E179" s="19" t="s">
+      <c r="E179" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A180" s="14"/>
-      <c r="B180" s="15"/>
-      <c r="C180" s="15"/>
-      <c r="D180" s="20" t="s">
+      <c r="A180" s="10"/>
+      <c r="D180" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E180" s="19" t="s">
+      <c r="E180" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A181" s="14"/>
-      <c r="B181" s="15"/>
-      <c r="C181" s="15"/>
-      <c r="D181" s="23" t="s">
+      <c r="A181" s="10"/>
+      <c r="D181" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E181" s="19" t="s">
+      <c r="E181" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A182" s="14"/>
-      <c r="B182" s="15"/>
-      <c r="C182" s="15"/>
-      <c r="D182" s="23" t="s">
+      <c r="A182" s="10"/>
+      <c r="D182" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E182" s="19" t="s">
+      <c r="E182" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A183" s="14"/>
-      <c r="B183" s="15"/>
-      <c r="C183" s="15"/>
-      <c r="D183" s="24" t="s">
+      <c r="A183" s="10"/>
+      <c r="D183" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E183" s="19" t="s">
+      <c r="E183" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A184" s="14"/>
-      <c r="B184" s="15"/>
-      <c r="C184" s="15"/>
-      <c r="D184" s="24" t="s">
+      <c r="A184" s="10"/>
+      <c r="D184" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E184" s="19" t="s">
+      <c r="E184" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A185" s="14"/>
-      <c r="B185" s="15"/>
-      <c r="C185" s="15" t="s">
+      <c r="A185" s="10"/>
+      <c r="C185" t="s">
         <v>58</v>
       </c>
-      <c r="D185" s="25" t="s">
+      <c r="D185" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E185" s="19" t="s">
+      <c r="E185" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A186" s="14"/>
-      <c r="B186" s="15"/>
-      <c r="C186" s="15"/>
-      <c r="D186" s="25" t="s">
+      <c r="A186" s="10"/>
+      <c r="D186" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E186" s="19" t="s">
+      <c r="E186" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A187" s="14"/>
-      <c r="B187" s="15"/>
-      <c r="C187" s="15"/>
-      <c r="D187" s="15" t="s">
+      <c r="A187" s="10"/>
+      <c r="D187" t="s">
         <v>6</v>
       </c>
-      <c r="E187" s="19" t="s">
+      <c r="E187" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A188" s="14"/>
-      <c r="B188" s="15"/>
-      <c r="C188" s="15"/>
-      <c r="D188" s="15" t="s">
+      <c r="A188" s="10"/>
+      <c r="D188" t="s">
         <v>7</v>
       </c>
-      <c r="E188" s="19" t="s">
+      <c r="E188" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A189" s="14"/>
-      <c r="B189" s="15"/>
-      <c r="C189" s="15"/>
-      <c r="D189" s="15" t="s">
+      <c r="A189" s="10"/>
+      <c r="D189" t="s">
         <v>2</v>
       </c>
-      <c r="E189" s="19" t="s">
+      <c r="E189" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A190" s="14"/>
-      <c r="B190" s="15"/>
-      <c r="C190" s="15"/>
-      <c r="D190" s="15" t="s">
+      <c r="A190" s="10"/>
+      <c r="D190" t="s">
         <v>8</v>
       </c>
-      <c r="E190" s="19" t="s">
+      <c r="E190" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A191" s="14"/>
-      <c r="B191" s="15"/>
-      <c r="C191" s="15"/>
-      <c r="D191" s="15" t="s">
+      <c r="A191" s="10"/>
+      <c r="D191" t="s">
         <v>9</v>
       </c>
-      <c r="E191" s="19" t="s">
+      <c r="E191" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A192" s="4"/>
-      <c r="B192" s="11"/>
-      <c r="C192" s="11"/>
-      <c r="D192" s="11" t="s">
+      <c r="A192" s="2"/>
+      <c r="B192" s="7"/>
+      <c r="C192" s="7"/>
+      <c r="D192" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E192" s="12" t="s">
+      <c r="E192" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A194" s="13" t="s">
+      <c r="A194" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B194" s="9"/>
-      <c r="C194" s="9"/>
-      <c r="D194" s="9" t="s">
+      <c r="B194" s="5"/>
+      <c r="C194" s="5"/>
+      <c r="D194" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E194" s="10" t="s">
+      <c r="E194" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A195" s="14"/>
-      <c r="B195" s="15"/>
-      <c r="C195" s="15"/>
-      <c r="D195" s="15" t="s">
+      <c r="A195" s="10"/>
+      <c r="D195" t="s">
         <v>1</v>
       </c>
-      <c r="E195" s="19" t="s">
+      <c r="E195" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A196" s="14"/>
-      <c r="B196" s="15"/>
-      <c r="C196" s="15"/>
-      <c r="D196" s="18" t="s">
+      <c r="A196" s="10"/>
+      <c r="D196" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E196" s="19" t="s">
+      <c r="E196" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A197" s="14"/>
-      <c r="B197" s="15"/>
-      <c r="C197" s="15"/>
-      <c r="D197" s="18" t="s">
+      <c r="A197" s="10"/>
+      <c r="D197" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E197" s="19" t="s">
+      <c r="E197" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A198" s="14"/>
-      <c r="B198" s="15"/>
-      <c r="C198" s="15"/>
-      <c r="D198" s="15" t="s">
+      <c r="A198" s="10"/>
+      <c r="D198" t="s">
         <v>3</v>
       </c>
-      <c r="E198" s="19" t="s">
+      <c r="E198" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A199" s="14"/>
-      <c r="B199" s="15"/>
-      <c r="C199" s="15"/>
-      <c r="D199" s="26" t="s">
+      <c r="A199" s="10"/>
+      <c r="D199" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E199" s="19" t="s">
+      <c r="E199" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A200" s="14"/>
-      <c r="B200" s="15"/>
-      <c r="C200" s="15"/>
-      <c r="D200" s="26" t="s">
+      <c r="A200" s="10"/>
+      <c r="D200" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E200" s="19" t="s">
+      <c r="E200" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A201" s="14"/>
-      <c r="B201" s="15"/>
-      <c r="C201" s="15"/>
-      <c r="D201" s="20" t="s">
+      <c r="A201" s="10"/>
+      <c r="D201" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E201" s="19" t="s">
+      <c r="E201" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A202" s="14"/>
-      <c r="B202" s="15"/>
-      <c r="C202" s="15"/>
-      <c r="D202" s="20" t="s">
+      <c r="A202" s="10"/>
+      <c r="D202" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E202" s="19" t="s">
+      <c r="E202" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A203" s="14"/>
-      <c r="B203" s="15"/>
-      <c r="C203" s="15"/>
-      <c r="D203" s="20" t="s">
+      <c r="A203" s="10"/>
+      <c r="D203" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E203" s="19" t="s">
+      <c r="E203" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A204" s="14"/>
-      <c r="B204" s="15"/>
-      <c r="C204" s="15"/>
-      <c r="D204" s="23" t="s">
+      <c r="A204" s="10"/>
+      <c r="D204" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E204" s="19" t="s">
+      <c r="E204" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A205" s="14"/>
-      <c r="B205" s="15"/>
-      <c r="C205" s="15"/>
-      <c r="D205" s="23" t="s">
+      <c r="A205" s="10"/>
+      <c r="D205" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E205" s="19" t="s">
+      <c r="E205" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A206" s="14"/>
-      <c r="B206" s="15"/>
-      <c r="C206" s="15"/>
-      <c r="D206" s="24" t="s">
+      <c r="A206" s="10"/>
+      <c r="D206" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E206" s="19" t="s">
+      <c r="E206" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A207" s="14"/>
-      <c r="B207" s="15"/>
-      <c r="C207" s="15"/>
-      <c r="D207" s="24" t="s">
+      <c r="A207" s="10"/>
+      <c r="D207" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E207" s="19" t="s">
+      <c r="E207" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A208" s="14"/>
-      <c r="B208" s="15"/>
-      <c r="C208" s="15"/>
-      <c r="D208" s="25" t="s">
+      <c r="A208" s="10"/>
+      <c r="D208" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E208" s="19" t="s">
+      <c r="E208" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A209" s="14"/>
-      <c r="B209" s="15"/>
-      <c r="C209" s="15"/>
-      <c r="D209" s="25" t="s">
+      <c r="A209" s="10"/>
+      <c r="D209" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E209" s="19" t="s">
+      <c r="E209" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A210" s="14"/>
-      <c r="B210" s="15"/>
-      <c r="C210" s="15"/>
-      <c r="D210" s="15" t="s">
+      <c r="A210" s="10"/>
+      <c r="D210" t="s">
         <v>6</v>
       </c>
-      <c r="E210" s="19" t="s">
+      <c r="E210" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A211" s="14"/>
-      <c r="B211" s="15"/>
-      <c r="C211" s="15"/>
-      <c r="D211" s="15" t="s">
+      <c r="A211" s="10"/>
+      <c r="D211" t="s">
         <v>7</v>
       </c>
-      <c r="E211" s="19" t="s">
+      <c r="E211" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A212" s="14"/>
-      <c r="B212" s="15"/>
-      <c r="C212" s="15"/>
-      <c r="D212" s="15" t="s">
+      <c r="A212" s="10"/>
+      <c r="D212" t="s">
         <v>2</v>
       </c>
-      <c r="E212" s="19" t="s">
+      <c r="E212" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A213" s="14"/>
-      <c r="B213" s="15"/>
-      <c r="C213" s="15"/>
-      <c r="D213" s="15" t="s">
+      <c r="A213" s="10"/>
+      <c r="D213" t="s">
         <v>8</v>
       </c>
-      <c r="E213" s="19" t="s">
+      <c r="E213" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A214" s="14"/>
-      <c r="B214" s="15"/>
-      <c r="C214" s="15"/>
-      <c r="D214" s="15" t="s">
+      <c r="A214" s="10"/>
+      <c r="D214" t="s">
         <v>9</v>
       </c>
-      <c r="E214" s="19" t="s">
+      <c r="E214" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A215" s="4"/>
-      <c r="B215" s="11"/>
-      <c r="C215" s="11"/>
-      <c r="D215" s="11" t="s">
+      <c r="A215" s="2"/>
+      <c r="B215" s="7"/>
+      <c r="C215" s="7"/>
+      <c r="D215" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E215" s="12" t="s">
+      <c r="E215" s="8" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>